<commit_message>
Correct xls file, correct autotask for Coaticook
</commit_message>
<xml_diff>
--- a/20221106-Projects Jerome.xlsx
+++ b/20221106-Projects Jerome.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://forgestik0-my.sharepoint.com/personal/jcholewa_forgestik_com/Documents/Documents/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="551" documentId="13_ncr:40009_{E1EA40D9-8353-4A57-9899-E0EE1F2B4E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{296160E9-7C83-4C23-9EFD-D79D50AE229C}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:40009_{E1EA40D9-8353-4A57-9899-E0EE1F2B4E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B795376-27A2-4D7C-8F50-A5B3EE92FB37}"/>
   <bookViews>
-    <workbookView xWindow="816" yWindow="264" windowWidth="21384" windowHeight="11532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="312" windowWidth="19524" windowHeight="11244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projets Jerome" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="238">
   <si>
     <t>Classification</t>
   </si>
@@ -786,6 +786,9 @@
   <si>
     <t>https://ww14.autotask.net/Mvc/Projects/ProjectDetail.mvc/ProjectDetail?gridConfiguration=Outline&amp;initialContentPage=Summary&amp;projectId=866</t>
   </si>
+  <si>
+    <t>https://ww14.autotask.net/Mvc/Projects/ProjectDetail.mvc/ProjectDetail?gridConfiguration=Outline&amp;initialContentPage=Summary&amp;projectId=840</t>
+  </si>
 </sst>
 </file>
 
@@ -794,7 +797,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,7 +1344,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1434,9 +1437,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1491,10 +1491,6 @@
   </cellStyles>
   <dxfs count="46">
     <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1524,6 +1520,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1699,21 +1699,21 @@
     <tableColumn id="9" xr3:uid="{FFFB7FDF-B233-4A10-8E95-9E28D56516C4}" name="Total Hours Worked" dataDxfId="13"/>
     <tableColumn id="15" xr3:uid="{0B8C6651-7292-4436-AF09-519B7A18F0CE}" name="Hourly rate" dataDxfId="12"/>
     <tableColumn id="16" xr3:uid="{B4B5896D-7653-4E8E-987F-DF39A1A99ADB}" name="Currency" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{4603F999-674A-4CEB-8FED-8845FE1510F9}" name="Estimated Revenue" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{4603F999-674A-4CEB-8FED-8845FE1510F9}" name="Estimated Revenue" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[Estimated Hours]]*Table1[[#This Row],[Hourly rate]]*1.15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7EC8EA46-BE08-4999-B2F1-17012169C257}" name="Project Number" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{EEC9B2F6-7BF8-47E5-853D-BE16CD95295C}" name="Contract" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{168F1290-19D5-4B2B-A00B-9E5E7A250B40}" name="ContractID" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{7EC8EA46-BE08-4999-B2F1-17012169C257}" name="Project Number" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{EEC9B2F6-7BF8-47E5-853D-BE16CD95295C}" name="Contract" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{168F1290-19D5-4B2B-A00B-9E5E7A250B40}" name="ContractID" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table13[[#This Row],[Project Number]],import!$J$2:$J$22,import!$N$2:$N$22)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{E169E80C-9F1A-4091-96BB-DF0CAB8BDFDA}" name="Create Date" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{3F2945AB-9DB4-424B-A969-8609F42AE8A8}" name="Account Manager" dataDxfId="6"/>
-    <tableColumn id="26" xr3:uid="{0C4ECDE9-C18D-4E11-9CE7-B41EE22BF6D8}" name="Location" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{B3FDF5BD-341D-4C3C-8CDD-E32B3544E203}" name="Lat" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{A189BBEE-A000-4D5B-9C0B-1AC5A4423DD3}" name="Long" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{11FC0B3C-D2D0-4B5C-9080-3BEE5E20C913}" name="Adresse" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{086159E6-9399-4330-B9F6-C2F8702E6E71}" name="Autotask" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{E169E80C-9F1A-4091-96BB-DF0CAB8BDFDA}" name="Create Date" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{3F2945AB-9DB4-424B-A969-8609F42AE8A8}" name="Account Manager" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{0C4ECDE9-C18D-4E11-9CE7-B41EE22BF6D8}" name="Location" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{B3FDF5BD-341D-4C3C-8CDD-E32B3544E203}" name="Lat" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{A189BBEE-A000-4D5B-9C0B-1AC5A4423DD3}" name="Long" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{11FC0B3C-D2D0-4B5C-9080-3BEE5E20C913}" name="Adresse" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{086159E6-9399-4330-B9F6-C2F8702E6E71}" name="Autotask" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2019,14 +2019,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView zoomScale="52" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="R7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -2057,7 +2057,7 @@
     <col min="28" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="13" customFormat="1" ht="28.8">
+    <row r="1" spans="1:27" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="15" customFormat="1">
+    <row r="2" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>Implantation SAP HANA Azure + We Go Trade</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="3" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>23</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>Implantation SAP SQL Produmex</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="4" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>Implantation Editions Chouette</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="5" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>42</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>Implementation SAP HANA Versago</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="6" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>42</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>Implantation WMS</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="7" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>42</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>Implantation WMS</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="15" customFormat="1">
+    <row r="8" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>CMBB SAP Implementation</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="15" customFormat="1">
+    <row r="9" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>Migration SAP V10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="15" customFormat="1">
+    <row r="10" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>42</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>Implantation Produmex Scan</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="11" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>42</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>SAP HANA Implementation</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="15" customFormat="1">
+    <row r="12" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>42</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>Migration V10 SQL</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="13" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>102</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>Implantation SAP phase 1 et 2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" s="15" customFormat="1">
+    <row r="14" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>Fixed assets implementation</v>
       </c>
     </row>
-    <row r="15" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="15" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>Implementation SAP HANA</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="16" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>Implantation SAP</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="17" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>42</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>Migration SAP V10 SQL</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="18" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>102</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>SAP V10 Migration</v>
       </c>
     </row>
-    <row r="19" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="19" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="20" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>102</v>
       </c>
@@ -3549,11 +3549,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="21" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="15" t="s">
         <v>139</v>
       </c>
       <c r="C21" s="15" t="s">
@@ -3621,11 +3621,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="15" customFormat="1" ht="43.2">
+    <row r="22" spans="1:27" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>234</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -3641,7 +3641,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="14">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14">
@@ -3652,9 +3652,9 @@
       </c>
       <c r="K22" s="17">
         <f>Table1[[#This Row],[Estimated Hours]]*Table1[[#This Row],[Hourly rate]]*1.15</f>
-        <v>8728.5</v>
-      </c>
-      <c r="L22" s="36" t="s">
+        <v>7969.4999999999991</v>
+      </c>
+      <c r="L22" s="35" t="s">
         <v>235</v>
       </c>
       <c r="M22" s="33" t="s">
@@ -3685,7 +3685,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="23" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>137</v>
       </c>
       <c r="U23" s="18" t="s">
-        <v>138</v>
+        <v>237</v>
       </c>
       <c r="Z23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Project Number]],import!$J$2:$J$24,import!$C$2:$C$24)</f>
@@ -3760,7 +3760,7 @@
         <v>Produmex WMS</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="24" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>23</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>Implantation SAP B1 &amp; Process Force</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="15" customFormat="1">
+    <row r="25" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>23</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>Projet implantation SAP et WMS</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="15" customFormat="1">
+    <row r="26" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>42</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>Dubois Agrinovations - Archivage</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="15" customFormat="1">
+    <row r="27" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C27" s="15" t="s">
         <v>182</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="15" customFormat="1">
+    <row r="28" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="15" t="s">
         <v>185</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="29" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C29" s="15" t="s">
         <v>188</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="15" customFormat="1" ht="28.8">
+    <row r="30" spans="1:27" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="15" t="s">
         <v>191</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="15" customFormat="1">
+    <row r="31" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="G31" s="14"/>
@@ -4157,7 +4157,7 @@
       <c r="Q31" s="18"/>
       <c r="T31" s="19"/>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="K32" s="5">
@@ -4171,7 +4171,7 @@
       <c r="O32" s="2"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="4:30">
+    <row r="33" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="K33" s="5">
@@ -4185,7 +4185,7 @@
       <c r="O33" s="2"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="4:30">
+    <row r="34" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="K34" s="5">
@@ -4199,7 +4199,7 @@
       <c r="O34" s="2"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="4:30">
+    <row r="35" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="K35" s="5">
@@ -4213,7 +4213,7 @@
       <c r="O35" s="2"/>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="4:30">
+    <row r="36" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="K36" s="5">
@@ -4227,7 +4227,7 @@
       <c r="O36" s="2"/>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="4:30">
+    <row r="37" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="K37" s="5">
@@ -4241,7 +4241,7 @@
       <c r="O37" s="2"/>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="4:30">
+    <row r="38" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="K38" s="5">
@@ -4255,7 +4255,7 @@
       <c r="O38" s="2"/>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="4:30">
+    <row r="39" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="K39" s="5">
@@ -4281,13 +4281,13 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="4:30" ht="21">
+    <row r="43" spans="4:30" ht="21" x14ac:dyDescent="0.3">
       <c r="F43" s="7" t="s">
         <v>196</v>
       </c>
       <c r="G43" s="8">
         <f>SUM(G2:G42)</f>
-        <v>6265</v>
+        <v>6261</v>
       </c>
       <c r="H43" s="8">
         <f>SUM(H2:H42)</f>
@@ -4297,7 +4297,7 @@
       <c r="J43" s="8"/>
       <c r="K43" s="9">
         <f>SUM(K2:K42)</f>
-        <v>1198731.25</v>
+        <v>1197972.25</v>
       </c>
       <c r="L43" s="8"/>
     </row>
@@ -4335,26 +4335,26 @@
     <hyperlink ref="U12" r:id="rId29" xr:uid="{56AC02A9-CDDC-48F6-A205-2F53E58CE26B}"/>
     <hyperlink ref="U8" r:id="rId30" xr:uid="{AC078D98-3E88-4FB8-BC94-8F60F49C0C3E}"/>
     <hyperlink ref="U17" r:id="rId31" xr:uid="{AE0926AF-0D4F-4175-8922-ADE5E63DEDC2}"/>
-    <hyperlink ref="U23" r:id="rId32" xr:uid="{1661FFF4-2BF8-4528-BA51-25951C50301B}"/>
-    <hyperlink ref="U11" r:id="rId33" xr:uid="{FCA5533E-ECBF-41F2-AE76-BECBB99AA3EA}"/>
-    <hyperlink ref="U9" r:id="rId34" xr:uid="{B36E3134-6C98-4F07-8B89-8C34E9546693}"/>
-    <hyperlink ref="U10" r:id="rId35" xr:uid="{F7697C27-23E1-46D7-A156-D9EBB9935C14}"/>
-    <hyperlink ref="U2" r:id="rId36" xr:uid="{EE6BC8DA-22DE-4CC4-A7DF-CCB1261F763D}"/>
-    <hyperlink ref="U26" r:id="rId37" xr:uid="{627DBD2C-06B8-456E-ACD8-680EC5579D25}"/>
-    <hyperlink ref="U4" r:id="rId38" xr:uid="{546CF0FA-5080-42E9-B7C6-A05D752DB590}"/>
-    <hyperlink ref="U20" r:id="rId39" xr:uid="{1A06EE69-A02F-4AD1-9841-3F56CBEE5324}"/>
-    <hyperlink ref="U18" r:id="rId40" xr:uid="{4E9D6236-4FA9-4892-970A-18063817DFA2}"/>
-    <hyperlink ref="U19" r:id="rId41" xr:uid="{E9594A89-30B1-40E5-BB84-805BCCCB82A0}"/>
-    <hyperlink ref="U13" r:id="rId42" xr:uid="{222A2A18-77BB-424D-BEE8-1AF6BCDBD7A5}"/>
-    <hyperlink ref="U21" r:id="rId43" xr:uid="{E8923AEC-D7E5-4E27-8D0D-2069DF864B54}"/>
-    <hyperlink ref="U15" r:id="rId44" xr:uid="{DCDC129F-53BE-4F51-A521-48EBB5492834}"/>
-    <hyperlink ref="U16" r:id="rId45" xr:uid="{128C8243-3300-43A2-8C41-9CC19D6328F1}"/>
-    <hyperlink ref="U5" r:id="rId46" xr:uid="{F165E2D2-FA93-462E-9F63-9A1F20C9B082}"/>
-    <hyperlink ref="U3" r:id="rId47" xr:uid="{237242D1-3594-4B74-A6E2-DEB86B8AD6D1}"/>
-    <hyperlink ref="U6" r:id="rId48" xr:uid="{901B818D-2C8B-48F8-9260-BA4664CB8B36}"/>
-    <hyperlink ref="U7" r:id="rId49" xr:uid="{FECCE0F5-11B9-432A-A29C-0E77399D40E6}"/>
-    <hyperlink ref="U14" r:id="rId50" xr:uid="{CA8AA73A-258E-495B-B927-A9B5C55093B6}"/>
-    <hyperlink ref="Q22" r:id="rId51" display="https://www.google.fr/maps/place/Produits+Electrolation+Inc/@45.594032,-73.7443942,19z/data=!4m12!1m6!3m5!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!2sProduits+Electrolation+Inc!8m2!3d45.5943373!4d-73.7441876!3m4!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!8m2!3d45.5943373!4d-73.7441876!5m1!1e1?hl=fr" xr:uid="{7680145A-3DE8-462D-81CC-AEF4F5D80B79}"/>
+    <hyperlink ref="U11" r:id="rId32" xr:uid="{FCA5533E-ECBF-41F2-AE76-BECBB99AA3EA}"/>
+    <hyperlink ref="U9" r:id="rId33" xr:uid="{B36E3134-6C98-4F07-8B89-8C34E9546693}"/>
+    <hyperlink ref="U10" r:id="rId34" xr:uid="{F7697C27-23E1-46D7-A156-D9EBB9935C14}"/>
+    <hyperlink ref="U2" r:id="rId35" xr:uid="{EE6BC8DA-22DE-4CC4-A7DF-CCB1261F763D}"/>
+    <hyperlink ref="U26" r:id="rId36" xr:uid="{627DBD2C-06B8-456E-ACD8-680EC5579D25}"/>
+    <hyperlink ref="U4" r:id="rId37" xr:uid="{546CF0FA-5080-42E9-B7C6-A05D752DB590}"/>
+    <hyperlink ref="U20" r:id="rId38" xr:uid="{1A06EE69-A02F-4AD1-9841-3F56CBEE5324}"/>
+    <hyperlink ref="U18" r:id="rId39" xr:uid="{4E9D6236-4FA9-4892-970A-18063817DFA2}"/>
+    <hyperlink ref="U19" r:id="rId40" xr:uid="{E9594A89-30B1-40E5-BB84-805BCCCB82A0}"/>
+    <hyperlink ref="U13" r:id="rId41" xr:uid="{222A2A18-77BB-424D-BEE8-1AF6BCDBD7A5}"/>
+    <hyperlink ref="U21" r:id="rId42" xr:uid="{E8923AEC-D7E5-4E27-8D0D-2069DF864B54}"/>
+    <hyperlink ref="U15" r:id="rId43" xr:uid="{DCDC129F-53BE-4F51-A521-48EBB5492834}"/>
+    <hyperlink ref="U16" r:id="rId44" xr:uid="{128C8243-3300-43A2-8C41-9CC19D6328F1}"/>
+    <hyperlink ref="U5" r:id="rId45" xr:uid="{F165E2D2-FA93-462E-9F63-9A1F20C9B082}"/>
+    <hyperlink ref="U3" r:id="rId46" xr:uid="{237242D1-3594-4B74-A6E2-DEB86B8AD6D1}"/>
+    <hyperlink ref="U6" r:id="rId47" xr:uid="{901B818D-2C8B-48F8-9260-BA4664CB8B36}"/>
+    <hyperlink ref="U7" r:id="rId48" xr:uid="{FECCE0F5-11B9-432A-A29C-0E77399D40E6}"/>
+    <hyperlink ref="U14" r:id="rId49" xr:uid="{CA8AA73A-258E-495B-B927-A9B5C55093B6}"/>
+    <hyperlink ref="Q22" r:id="rId50" display="https://www.google.fr/maps/place/Produits+Electrolation+Inc/@45.594032,-73.7443942,19z/data=!4m12!1m6!3m5!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!2sProduits+Electrolation+Inc!8m2!3d45.5943373!4d-73.7441876!3m4!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!8m2!3d45.5943373!4d-73.7441876!5m1!1e1?hl=fr" xr:uid="{7680145A-3DE8-462D-81CC-AEF4F5D80B79}"/>
+    <hyperlink ref="U23" r:id="rId51" xr:uid="{21279F06-E318-4546-B7D1-03A7336EA700}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId52"/>
@@ -4376,7 +4376,7 @@
       <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" style="4" bestFit="1" customWidth="1"/>
@@ -4394,7 +4394,7 @@
     <col min="15" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>CMBB Bakeware Canada Inc.</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>Coco Bakery Inc.</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>Cowper Inc.</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>Cowper Inc.</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>206</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>Distribution GVA</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>Dubois Agrinovation Inc.</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>Éditions Chouette</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>Entreprise Tenzo inc.</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>102</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>Federal Steel Equipment Ltd.</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>206</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>Fromagerie Polyethnique Inc</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>102</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>Gazebo Penguin Inc.</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>206</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>Groupe Carreaux Céragrès Inc.</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>Laiterie de Coaticook ltée</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>Laiterie de Coaticook ltée</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>Les Aliments CDS inc.</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>206</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>Lovato Electric Inc. (USA)</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>Megastar Électroniques Inc.</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>O&amp;T Farms</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>206</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>SIT Mauricie</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>Tzanet</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
@@ -5459,14 +5459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77C97A1-5E5F-426D-9D38-9B71B1F2530B}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q9" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="U17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="AH23" sqref="AH23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="15" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" style="15" bestFit="1" customWidth="1"/>
@@ -5491,7 +5491,7 @@
     <col min="21" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="13" customFormat="1" ht="28.8">
+    <row r="1" spans="1:21" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="28.8">
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>23</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="28.8">
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>42</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="28.8">
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>42</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="28.8">
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>42</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>42</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.8">
+    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>42</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>42</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="28.8">
+    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>102</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>42</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="28.8">
+    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.8">
+    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="28.8">
+    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>42</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="28.8">
+    <row r="18" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>102</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="28.8">
+    <row r="19" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="28.8">
+    <row r="20" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>102</v>
       </c>
@@ -6807,11 +6807,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="28.8">
+    <row r="21" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="15" t="s">
         <v>139</v>
       </c>
       <c r="C21" s="15" t="s">
@@ -6870,11 +6870,11 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="43.2">
+    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>234</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -6900,9 +6900,9 @@
       </c>
       <c r="K22" s="17">
         <f>Table1[[#This Row],[Estimated Hours]]*Table1[[#This Row],[Hourly rate]]*1.15</f>
-        <v>8728.5</v>
-      </c>
-      <c r="L22" s="36" t="s">
+        <v>7969.4999999999991</v>
+      </c>
+      <c r="L22" s="35" t="s">
         <v>235</v>
       </c>
       <c r="M22" s="33" t="s">
@@ -6933,7 +6933,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="28.8">
+    <row r="23" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
@@ -6996,10 +6996,10 @@
         <v>137</v>
       </c>
       <c r="U23" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="28.8">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>23</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>23</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>42</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C27" s="15" t="s">
         <v>182</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C28" s="15" t="s">
         <v>185</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="28.8">
+    <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C29" s="15" t="s">
         <v>188</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="28.8">
+    <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="15" t="s">
         <v>191</v>
       </c>
@@ -7326,26 +7326,26 @@
     <hyperlink ref="U12" r:id="rId28" xr:uid="{63252B0E-968D-4903-85E9-AE26C020D1C7}"/>
     <hyperlink ref="U8" r:id="rId29" xr:uid="{15C9796E-B70B-477A-8C97-57BA71FB77B7}"/>
     <hyperlink ref="U17" r:id="rId30" xr:uid="{4A619612-2B71-498A-ABCF-8C99B29DD011}"/>
-    <hyperlink ref="U23" r:id="rId31" xr:uid="{0B855394-43C2-40E1-A7E8-D8A617EC3BF7}"/>
-    <hyperlink ref="U11" r:id="rId32" xr:uid="{8144DB44-4A3D-4EE9-BC66-DCF6985C1389}"/>
-    <hyperlink ref="U9" r:id="rId33" xr:uid="{0F3CAF0E-D472-4CFF-A59E-36F93C514F31}"/>
-    <hyperlink ref="U10" r:id="rId34" xr:uid="{A9BE4C8D-9B3F-4B59-81B1-B27BB5B0101B}"/>
-    <hyperlink ref="U2" r:id="rId35" xr:uid="{E97220D9-0FDA-435A-A97E-1C814244BA51}"/>
-    <hyperlink ref="U26" r:id="rId36" xr:uid="{F8080523-A57B-42F2-B75C-79BB5CE59A74}"/>
-    <hyperlink ref="U4" r:id="rId37" xr:uid="{4C447D64-4252-46FD-8DEB-664F14891728}"/>
-    <hyperlink ref="U20" r:id="rId38" xr:uid="{4F2026DB-7B33-4E1B-9156-D271E6CC2001}"/>
-    <hyperlink ref="U18" r:id="rId39" xr:uid="{6439A4DC-A6D4-4F69-A269-9BCAE60DCB0C}"/>
-    <hyperlink ref="U19" r:id="rId40" xr:uid="{C276DADC-3515-44F8-9906-F7C0458497BC}"/>
-    <hyperlink ref="U13" r:id="rId41" xr:uid="{F8A58757-361C-487F-A7FE-BC99C9F056AB}"/>
-    <hyperlink ref="U21" r:id="rId42" xr:uid="{A4A9CC2E-7D8C-4B19-A473-DA652DA2A3F2}"/>
-    <hyperlink ref="U15" r:id="rId43" xr:uid="{1C19E2B7-802C-4A23-86A7-B5490C4D974D}"/>
-    <hyperlink ref="U16" r:id="rId44" xr:uid="{BD8F9356-6F9D-49FB-9260-862D66144BEE}"/>
-    <hyperlink ref="U5" r:id="rId45" xr:uid="{5F214BBD-354C-47D4-90A4-B25C3A2CBD64}"/>
-    <hyperlink ref="U3" r:id="rId46" xr:uid="{B37C2440-3F37-45E2-AFE3-589A1835DA83}"/>
-    <hyperlink ref="U6" r:id="rId47" xr:uid="{4F4C3A78-4A4C-4BE7-896B-81CF2C8B6458}"/>
-    <hyperlink ref="U7" r:id="rId48" xr:uid="{396406FC-0BA6-4D94-93AD-0D5ADEDBB037}"/>
-    <hyperlink ref="U14" r:id="rId49" xr:uid="{113F999D-ACC9-4AB6-A6AB-8975BCEC01D2}"/>
-    <hyperlink ref="Q22" r:id="rId50" display="https://www.google.fr/maps/place/Produits+Electrolation+Inc/@45.594032,-73.7443942,19z/data=!4m12!1m6!3m5!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!2sProduits+Electrolation+Inc!8m2!3d45.5943373!4d-73.7441876!3m4!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!8m2!3d45.5943373!4d-73.7441876!5m1!1e1?hl=fr" xr:uid="{E0E4E55E-CCEB-4C94-97F3-C49BCEE74DD5}"/>
+    <hyperlink ref="U11" r:id="rId31" xr:uid="{8144DB44-4A3D-4EE9-BC66-DCF6985C1389}"/>
+    <hyperlink ref="U9" r:id="rId32" xr:uid="{0F3CAF0E-D472-4CFF-A59E-36F93C514F31}"/>
+    <hyperlink ref="U10" r:id="rId33" xr:uid="{A9BE4C8D-9B3F-4B59-81B1-B27BB5B0101B}"/>
+    <hyperlink ref="U2" r:id="rId34" xr:uid="{E97220D9-0FDA-435A-A97E-1C814244BA51}"/>
+    <hyperlink ref="U26" r:id="rId35" xr:uid="{F8080523-A57B-42F2-B75C-79BB5CE59A74}"/>
+    <hyperlink ref="U4" r:id="rId36" xr:uid="{4C447D64-4252-46FD-8DEB-664F14891728}"/>
+    <hyperlink ref="U20" r:id="rId37" xr:uid="{4F2026DB-7B33-4E1B-9156-D271E6CC2001}"/>
+    <hyperlink ref="U18" r:id="rId38" xr:uid="{6439A4DC-A6D4-4F69-A269-9BCAE60DCB0C}"/>
+    <hyperlink ref="U19" r:id="rId39" xr:uid="{C276DADC-3515-44F8-9906-F7C0458497BC}"/>
+    <hyperlink ref="U13" r:id="rId40" xr:uid="{F8A58757-361C-487F-A7FE-BC99C9F056AB}"/>
+    <hyperlink ref="U21" r:id="rId41" xr:uid="{A4A9CC2E-7D8C-4B19-A473-DA652DA2A3F2}"/>
+    <hyperlink ref="U15" r:id="rId42" xr:uid="{1C19E2B7-802C-4A23-86A7-B5490C4D974D}"/>
+    <hyperlink ref="U16" r:id="rId43" xr:uid="{BD8F9356-6F9D-49FB-9260-862D66144BEE}"/>
+    <hyperlink ref="U5" r:id="rId44" xr:uid="{5F214BBD-354C-47D4-90A4-B25C3A2CBD64}"/>
+    <hyperlink ref="U3" r:id="rId45" xr:uid="{B37C2440-3F37-45E2-AFE3-589A1835DA83}"/>
+    <hyperlink ref="U6" r:id="rId46" xr:uid="{4F4C3A78-4A4C-4BE7-896B-81CF2C8B6458}"/>
+    <hyperlink ref="U7" r:id="rId47" xr:uid="{396406FC-0BA6-4D94-93AD-0D5ADEDBB037}"/>
+    <hyperlink ref="U14" r:id="rId48" xr:uid="{113F999D-ACC9-4AB6-A6AB-8975BCEC01D2}"/>
+    <hyperlink ref="Q22" r:id="rId49" display="https://www.google.fr/maps/place/Produits+Electrolation+Inc/@45.594032,-73.7443942,19z/data=!4m12!1m6!3m5!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!2sProduits+Electrolation+Inc!8m2!3d45.5943373!4d-73.7441876!3m4!1s0x4cc92143ec29647d:0x9f89ab8988471bbd!8m2!3d45.5943373!4d-73.7441876!5m1!1e1?hl=fr" xr:uid="{E0E4E55E-CCEB-4C94-97F3-C49BCEE74DD5}"/>
+    <hyperlink ref="U23" r:id="rId50" xr:uid="{3EEE83CF-B9B5-40BB-8F69-0239421DABA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId51"/>

</xml_diff>